<commit_message>
DJS - Updated HW11 Code and Added LinElast
</commit_message>
<xml_diff>
--- a/2DBVP/Figures/HW11_Torque.xlsx
+++ b/2DBVP/Figures/HW11_Torque.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>square</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>quarter circle</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>Step Diff</t>
   </si>
 </sst>
 </file>
@@ -363,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,6 +493,106 @@
         <v>16.256</v>
       </c>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>38.510800000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>40.344999999999999</v>
+      </c>
+      <c r="D11">
+        <f>C11-C10</f>
+        <v>1.8341999999999956</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>40</v>
+      </c>
+      <c r="C12">
+        <v>42.182600000000001</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:D15" si="0">C12-C11</f>
+        <v>1.8376000000000019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>32</v>
+      </c>
+      <c r="B13">
+        <v>80</v>
+      </c>
+      <c r="C13">
+        <v>44.021000000000001</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1.8384</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>64</v>
+      </c>
+      <c r="B14">
+        <v>160</v>
+      </c>
+      <c r="C14">
+        <v>45.859499999999997</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>1.8384999999999962</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>96</v>
+      </c>
+      <c r="B15">
+        <v>240</v>
+      </c>
+      <c r="C15">
+        <v>46.935000000000002</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1.0755000000000052</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>